<commit_message>
Deploying to gh-pages from  @ 3ea501369c914b10a427e20b17cd26e4c079a0ea 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/15.1.2.xlsx
+++ b/en/downloads/data-excel/15.1.2.xlsx
@@ -164,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -204,6 +204,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +530,7 @@
     <col min="6" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -544,7 +547,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
@@ -555,7 +558,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -583,8 +586,14 @@
       <c r="I3" s="12">
         <v>2018</v>
       </c>
+      <c r="J3" s="12">
+        <v>2019</v>
+      </c>
+      <c r="K3" s="12">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
@@ -612,8 +621,14 @@
       <c r="I4" s="14">
         <v>7.38</v>
       </c>
+      <c r="J4" s="15">
+        <v>6.18</v>
+      </c>
+      <c r="K4" s="15">
+        <v>6.18</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -624,7 +639,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -635,7 +650,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>

</xml_diff>